<commit_message>
when Compare, it now accepts compare method. also add tests for bad data
</commit_message>
<xml_diff>
--- a/tests/data/compare_new1.xlsx
+++ b/tests/data/compare_new1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="960" windowWidth="24640" windowHeight="14560" tabRatio="500"/>
+    <workbookView xWindow="9720" yWindow="220" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>key</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>…æ</t>
+  </si>
+  <si>
+    <t>VQSR</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -450,7 +459,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -489,7 +498,10 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>17</v>
+      </c>
+      <c r="F2">
+        <v>0.3</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -505,6 +517,9 @@
       <c r="D3" t="s">
         <v>13</v>
       </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="16">
       <c r="A4">
@@ -519,6 +534,9 @@
       <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
@@ -534,7 +552,10 @@
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c r="F5">
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -549,6 +570,12 @@
       </c>
       <c r="D6" t="s">
         <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6">
+        <v>2.9999999999999997E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>